<commit_message>
added functionality, new data
</commit_message>
<xml_diff>
--- a/FantasyTeamPoints.xlsx
+++ b/FantasyTeamPoints.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mackenziewilson/Desktop/FantasyTeamBuilder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mackenziewilson/Desktop/CodeProjects/FantasyTeamBuilder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61083948-8311-F648-8E09-74CD29CCB1DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8D6E61-E004-2D43-9F56-0229B203E6FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00168D69-C4C6-6E49-BB3F-101C783196B4}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{00168D69-C4C6-6E49-BB3F-101C783196B4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Oct24Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Nov05Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="55">
   <si>
     <t>position_1</t>
   </si>
@@ -157,6 +158,39 @@
   </si>
   <si>
     <t>games_this_week</t>
+  </si>
+  <si>
+    <t>Monahan</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Gourde</t>
+  </si>
+  <si>
+    <t>Ekholm</t>
+  </si>
+  <si>
+    <t>Suter</t>
+  </si>
+  <si>
+    <t>Seabrook</t>
+  </si>
+  <si>
+    <t>CGY</t>
+  </si>
+  <si>
+    <t>NYI</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>NJ</t>
   </si>
 </sst>
 </file>
@@ -511,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50AE61DD-2226-0342-BA67-1E715A8202A0}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1085,4 +1119,594 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D283F34-C7C9-A94E-A068-D29254E8416F}">
+  <dimension ref="A1:L17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1">
+        <v>61</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1">
+        <v>61</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1">
+        <v>111.8</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1">
+        <v>78.7</v>
+      </c>
+      <c r="I3">
+        <v>14</v>
+      </c>
+      <c r="J3" s="1">
+        <v>139.19999999999999</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>46.1</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="I4">
+        <v>14</v>
+      </c>
+      <c r="J4" s="1">
+        <v>163.19999999999999</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>29.3</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5" s="1">
+        <v>87.5</v>
+      </c>
+      <c r="I5">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1">
+        <v>135.30000000000001</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>51.5</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6" s="1">
+        <v>62</v>
+      </c>
+      <c r="I6">
+        <v>14</v>
+      </c>
+      <c r="J6" s="1">
+        <v>124.6</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>37.6</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" s="1">
+        <v>79</v>
+      </c>
+      <c r="I7">
+        <v>13</v>
+      </c>
+      <c r="J7" s="1">
+        <v>119</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1">
+        <v>28.6</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8" s="1">
+        <v>42.2</v>
+      </c>
+      <c r="I8">
+        <v>13</v>
+      </c>
+      <c r="J8" s="1">
+        <v>93.8</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="H9" s="1">
+        <v>27</v>
+      </c>
+      <c r="I9">
+        <v>13</v>
+      </c>
+      <c r="J9" s="1">
+        <v>84.7</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1">
+        <v>21.5</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1">
+        <v>39</v>
+      </c>
+      <c r="I10">
+        <v>12</v>
+      </c>
+      <c r="J10" s="1">
+        <v>107.8</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1">
+        <v>17.3</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+      <c r="H11" s="1">
+        <v>52.9</v>
+      </c>
+      <c r="I11">
+        <v>14</v>
+      </c>
+      <c r="J11" s="1">
+        <v>89</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1">
+        <v>26.7</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+      <c r="H12" s="1">
+        <v>46.1</v>
+      </c>
+      <c r="I12">
+        <v>13</v>
+      </c>
+      <c r="J12" s="1">
+        <v>141.6</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
+      </c>
+      <c r="H13" s="1">
+        <v>58.9</v>
+      </c>
+      <c r="I13">
+        <v>13</v>
+      </c>
+      <c r="J13" s="1">
+        <v>151.19999999999999</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14" s="1">
+        <v>38.5</v>
+      </c>
+      <c r="I14">
+        <v>11</v>
+      </c>
+      <c r="J14" s="1">
+        <v>105.4</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15" s="1">
+        <v>34.1</v>
+      </c>
+      <c r="I15">
+        <v>10</v>
+      </c>
+      <c r="J15" s="1">
+        <v>84.2</v>
+      </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>21.8</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16" s="1">
+        <v>49.6</v>
+      </c>
+      <c r="I16">
+        <v>10</v>
+      </c>
+      <c r="J16" s="1">
+        <v>92</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" s="1">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="H17" s="1">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="I17">
+        <v>9</v>
+      </c>
+      <c r="J17" s="1">
+        <v>102.4</v>
+      </c>
+      <c r="K17">
+        <v>4</v>
+      </c>
+      <c r="L17" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new data, slight code changes
</commit_message>
<xml_diff>
--- a/FantasyTeamPoints.xlsx
+++ b/FantasyTeamPoints.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mackenziewilson/Desktop/CodeProjects/FantasyTeamBuilder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008DF4E3-AB83-9F45-AA80-6DC72F0AF7D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C29AD3-286B-F64C-8B69-4D12B8257497}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{00168D69-C4C6-6E49-BB3F-101C783196B4}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="4" xr2:uid="{00168D69-C4C6-6E49-BB3F-101C783196B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Oct24Data" sheetId="1" r:id="rId1"/>
     <sheet name="Nov05Data" sheetId="2" r:id="rId2"/>
     <sheet name="Nov12Data" sheetId="3" r:id="rId3"/>
+    <sheet name="Nov19Data" sheetId="4" r:id="rId4"/>
+    <sheet name="Nov26Data" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="61">
   <si>
     <t>position_1</t>
   </si>
@@ -195,6 +197,21 @@
   </si>
   <si>
     <t>TBL</t>
+  </si>
+  <si>
+    <t>games_total</t>
+  </si>
+  <si>
+    <t>points_total</t>
+  </si>
+  <si>
+    <t>Parise</t>
+  </si>
+  <si>
+    <t>Pionk</t>
+  </si>
+  <si>
+    <t>NYR</t>
   </si>
 </sst>
 </file>
@@ -1719,8 +1736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86519B51-FB1D-A541-86E3-CCE03A9F9D1E}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2287,4 +2304,1146 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D654F9-FC04-8C4D-950F-2DF18E7A9C48}">
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1">
+        <v>26.1</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1">
+        <v>53.4</v>
+      </c>
+      <c r="I2">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1">
+        <v>177.1</v>
+      </c>
+      <c r="K2">
+        <v>20</v>
+      </c>
+      <c r="L2" s="1">
+        <v>216.4</v>
+      </c>
+      <c r="M2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1">
+        <v>34</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1">
+        <v>46.3</v>
+      </c>
+      <c r="I3">
+        <v>14</v>
+      </c>
+      <c r="J3" s="1">
+        <v>133.30000000000001</v>
+      </c>
+      <c r="K3">
+        <v>20</v>
+      </c>
+      <c r="L3" s="1">
+        <v>214.9</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>46.1</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+      <c r="J4" s="1">
+        <v>120</v>
+      </c>
+      <c r="K4">
+        <v>20</v>
+      </c>
+      <c r="L4" s="1">
+        <v>212.7</v>
+      </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>10.6</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" s="1">
+        <v>60.4</v>
+      </c>
+      <c r="I5">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1">
+        <v>149.30000000000001</v>
+      </c>
+      <c r="K5">
+        <v>18</v>
+      </c>
+      <c r="L5" s="1">
+        <v>194.2</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>20.9</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6" s="1">
+        <v>63</v>
+      </c>
+      <c r="I6">
+        <v>13</v>
+      </c>
+      <c r="J6" s="1">
+        <v>99.4</v>
+      </c>
+      <c r="K6">
+        <v>20</v>
+      </c>
+      <c r="L6" s="1">
+        <v>187</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>25.1</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7" s="1">
+        <v>59.4</v>
+      </c>
+      <c r="I7">
+        <v>12</v>
+      </c>
+      <c r="J7" s="1">
+        <v>93.5</v>
+      </c>
+      <c r="K7">
+        <v>19</v>
+      </c>
+      <c r="L7" s="1">
+        <v>173.2</v>
+      </c>
+      <c r="M7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="I8">
+        <v>13</v>
+      </c>
+      <c r="J8" s="1">
+        <v>117.7</v>
+      </c>
+      <c r="K8">
+        <v>20</v>
+      </c>
+      <c r="L8" s="1">
+        <v>173.1</v>
+      </c>
+      <c r="M8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9" s="1">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="I9">
+        <v>14</v>
+      </c>
+      <c r="J9" s="1">
+        <v>109.1</v>
+      </c>
+      <c r="K9">
+        <v>19</v>
+      </c>
+      <c r="L9" s="1">
+        <v>169.5</v>
+      </c>
+      <c r="M9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1">
+        <v>11.8</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="H10" s="1">
+        <v>31.1</v>
+      </c>
+      <c r="I10">
+        <v>11</v>
+      </c>
+      <c r="J10" s="1">
+        <v>92.1</v>
+      </c>
+      <c r="K10">
+        <v>16</v>
+      </c>
+      <c r="L10" s="1">
+        <v>158.80000000000001</v>
+      </c>
+      <c r="M10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1">
+        <v>24.1</v>
+      </c>
+      <c r="G11">
+        <v>6</v>
+      </c>
+      <c r="H11" s="1">
+        <v>42.2</v>
+      </c>
+      <c r="I11">
+        <v>15</v>
+      </c>
+      <c r="J11" s="1">
+        <v>116</v>
+      </c>
+      <c r="K11">
+        <v>21</v>
+      </c>
+      <c r="L11" s="1">
+        <v>146.9</v>
+      </c>
+      <c r="M11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" s="1">
+        <v>24.7</v>
+      </c>
+      <c r="G12">
+        <v>6</v>
+      </c>
+      <c r="H12" s="1">
+        <v>33.4</v>
+      </c>
+      <c r="I12">
+        <v>13</v>
+      </c>
+      <c r="J12" s="1">
+        <v>81.3</v>
+      </c>
+      <c r="K12">
+        <v>20</v>
+      </c>
+      <c r="L12" s="1">
+        <v>136.19999999999999</v>
+      </c>
+      <c r="M12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1">
+        <v>30.6</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
+      </c>
+      <c r="H13" s="1">
+        <v>56.1</v>
+      </c>
+      <c r="I13">
+        <v>13</v>
+      </c>
+      <c r="J13" s="1">
+        <v>105.5</v>
+      </c>
+      <c r="K13">
+        <v>18</v>
+      </c>
+      <c r="L13" s="1">
+        <v>133.80000000000001</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14" s="1">
+        <v>12.6</v>
+      </c>
+      <c r="G14">
+        <v>6</v>
+      </c>
+      <c r="H14" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="I14">
+        <v>13</v>
+      </c>
+      <c r="J14" s="1">
+        <v>72.3</v>
+      </c>
+      <c r="K14">
+        <v>20</v>
+      </c>
+      <c r="L14" s="1">
+        <v>128</v>
+      </c>
+      <c r="M14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="G15">
+        <v>8</v>
+      </c>
+      <c r="H15" s="1">
+        <v>20.2</v>
+      </c>
+      <c r="I15">
+        <v>14</v>
+      </c>
+      <c r="J15" s="1">
+        <v>62.2</v>
+      </c>
+      <c r="K15">
+        <v>21</v>
+      </c>
+      <c r="L15" s="1">
+        <v>126.9</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>18.2</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16" s="1">
+        <v>53.4</v>
+      </c>
+      <c r="I16">
+        <v>8</v>
+      </c>
+      <c r="J16" s="1">
+        <v>103</v>
+      </c>
+      <c r="K16">
+        <v>14</v>
+      </c>
+      <c r="L16" s="1">
+        <v>172</v>
+      </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17" s="1">
+        <v>56.4</v>
+      </c>
+      <c r="I17">
+        <v>9</v>
+      </c>
+      <c r="J17" s="1">
+        <v>125</v>
+      </c>
+      <c r="K17">
+        <v>14</v>
+      </c>
+      <c r="L17" s="1">
+        <v>186.8</v>
+      </c>
+      <c r="M17">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6432FDE3-A129-F843-A862-67C4B57A6FA5}">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>45.6</v>
+      </c>
+      <c r="G2">
+        <v>24</v>
+      </c>
+      <c r="H2">
+        <v>262</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>30.7</v>
+      </c>
+      <c r="G3">
+        <v>24</v>
+      </c>
+      <c r="H3">
+        <v>243.4</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>19.5</v>
+      </c>
+      <c r="G4">
+        <v>23</v>
+      </c>
+      <c r="H4">
+        <v>234.4</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>25.8</v>
+      </c>
+      <c r="G5">
+        <v>22</v>
+      </c>
+      <c r="H5">
+        <v>220</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>43.9</v>
+      </c>
+      <c r="G6">
+        <v>24</v>
+      </c>
+      <c r="H6">
+        <v>217</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="G7">
+        <v>22</v>
+      </c>
+      <c r="H7">
+        <v>207.2</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>27.7</v>
+      </c>
+      <c r="G8">
+        <v>23</v>
+      </c>
+      <c r="H8">
+        <v>200.9</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>13.7</v>
+      </c>
+      <c r="G9">
+        <v>22</v>
+      </c>
+      <c r="H9">
+        <v>200.7</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>30.6</v>
+      </c>
+      <c r="G10">
+        <v>20</v>
+      </c>
+      <c r="H10">
+        <v>189.4</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>25</v>
+      </c>
+      <c r="G11">
+        <v>24</v>
+      </c>
+      <c r="H11">
+        <v>161.19999999999999</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>12.8</v>
+      </c>
+      <c r="G12">
+        <v>24</v>
+      </c>
+      <c r="H12">
+        <v>159.69999999999999</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>31.3</v>
+      </c>
+      <c r="G13">
+        <v>24</v>
+      </c>
+      <c r="H13">
+        <v>159.30000000000001</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <v>24.4</v>
+      </c>
+      <c r="G14">
+        <v>22</v>
+      </c>
+      <c r="H14">
+        <v>158.19999999999999</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>30.4</v>
+      </c>
+      <c r="G15">
+        <v>23</v>
+      </c>
+      <c r="H15">
+        <v>157.30000000000001</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>4.2</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>191</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>15.8</v>
+      </c>
+      <c r="G17">
+        <v>17</v>
+      </c>
+      <c r="H17">
+        <v>187.8</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New data and error handling
</commit_message>
<xml_diff>
--- a/FantasyTeamPoints.xlsx
+++ b/FantasyTeamPoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mackenziewilson/Desktop/CodeProjects/FantasyTeamBuilder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5514121-D091-2B45-A003-243869C556B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3F1DDB-DDB8-8340-BBA3-CE82769BDBEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00168D69-C4C6-6E49-BB3F-101C783196B4}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="5" xr2:uid="{00168D69-C4C6-6E49-BB3F-101C783196B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Oct24Data" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Nov12Data" sheetId="3" r:id="rId3"/>
     <sheet name="Nov19Data" sheetId="4" r:id="rId4"/>
     <sheet name="Nov26Data" sheetId="5" r:id="rId5"/>
+    <sheet name="Dec03Data" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="57">
   <si>
     <t>position_1</t>
   </si>
@@ -554,7 +555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50AE61DD-2226-0342-BA67-1E715A8202A0}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -2462,7 +2463,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2924,4 +2925,473 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE496352-635F-174E-B92B-B404BE4B139E}">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1">
+        <v>44.7</v>
+      </c>
+      <c r="G2">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1">
+        <v>288.10000000000002</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1">
+        <v>18.7</v>
+      </c>
+      <c r="G3">
+        <v>27</v>
+      </c>
+      <c r="H3" s="1">
+        <v>280.7</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>47.8</v>
+      </c>
+      <c r="G4">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1">
+        <v>267.8</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>63.1</v>
+      </c>
+      <c r="G5">
+        <v>26</v>
+      </c>
+      <c r="H5" s="1">
+        <v>264</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="G6">
+        <v>27</v>
+      </c>
+      <c r="H6" s="1">
+        <v>244.6</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>25.7</v>
+      </c>
+      <c r="G7">
+        <v>27</v>
+      </c>
+      <c r="H7" s="1">
+        <v>242.7</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1">
+        <v>26.9</v>
+      </c>
+      <c r="G8">
+        <v>25</v>
+      </c>
+      <c r="H8" s="1">
+        <v>234.1</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1">
+        <v>26.1</v>
+      </c>
+      <c r="G9">
+        <v>25</v>
+      </c>
+      <c r="H9" s="1">
+        <v>226.8</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="G10">
+        <v>23</v>
+      </c>
+      <c r="H10" s="1">
+        <v>196.1</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1">
+        <v>20.7</v>
+      </c>
+      <c r="G11">
+        <v>26</v>
+      </c>
+      <c r="H11" s="1">
+        <v>178</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="G12">
+        <v>27</v>
+      </c>
+      <c r="H12" s="1">
+        <v>177.9</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13" s="1">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="G13">
+        <v>26</v>
+      </c>
+      <c r="H13" s="1">
+        <v>176.6</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1">
+        <v>10.3</v>
+      </c>
+      <c r="G14">
+        <v>27</v>
+      </c>
+      <c r="H14" s="1">
+        <v>171.5</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15" s="1">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="G15">
+        <v>28</v>
+      </c>
+      <c r="H15" s="1">
+        <v>168.4</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16" s="1">
+        <v>14.8</v>
+      </c>
+      <c r="G16">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1">
+        <v>202.6</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="G17">
+        <v>16</v>
+      </c>
+      <c r="H17" s="1">
+        <v>207.4</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>